<commit_message>
adapt models fixed and tests
</commit_message>
<xml_diff>
--- a/output/adapt_forest_one_item_400_2.xlsx
+++ b/output/adapt_forest_one_item_400_2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,42 +451,102 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>MSE_transfer_rt</t>
+          <t>MSE_transfer_coral</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>MSE_transfer_sa</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>MSE_transfer_bw</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>MSE_transfer_nnw</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>MAE_no_transfer</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>MAE_transfer_basic</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>MAE_transfer_rt</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_transfer_coral</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_transfer_sa</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_transfer_bw</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_transfer_nnw</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>MSE_diff_basic</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>MSE_diff_rt</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>MSE_transfer_coral</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>MSE_diff_sa</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>MSE_diff_bw</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>MSE_diff_nnw</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>MAE_diff_basic</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>MAE_diff_rt</t>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_transfer_coral</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_diff_sa</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_diff_bw</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_diff_nnw</t>
         </is>
       </c>
     </row>
@@ -497,34 +557,70 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.22285909309842</v>
+        <v>1.222218837026467</v>
       </c>
       <c r="C2" t="n">
-        <v>1.061749863997642</v>
+        <v>1.063419466375333</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9598325237132443</v>
+        <v>1.111192752731464</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5128600489873809</v>
+        <v>1.020436886935692</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6087278243844356</v>
+        <v>0.8775133364974671</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3858387057351976</v>
+        <v>0.9284918576178334</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.1611092291007783</v>
+        <v>0.5127839979635104</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.2630265693851759</v>
+        <v>0.6062345606259164</v>
       </c>
       <c r="J2" t="n">
-        <v>0.09586777539705471</v>
+        <v>0.5632716150102758</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.1270213432521833</v>
+        <v>0.7701338342334212</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.4411453296771398</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.4037414647687326</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-0.1587993706511339</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-0.111026084295003</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-0.2017819500907749</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-0.3447055005290002</v>
+      </c>
+      <c r="R2" t="n">
+        <v>-0.2937269794086339</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.09345056266240603</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.05048761704676541</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.2573498362699108</v>
+      </c>
+      <c r="V2" t="n">
+        <v>-0.07163866828637061</v>
+      </c>
+      <c r="W2" t="n">
+        <v>-0.1090425331947777</v>
       </c>
     </row>
     <row r="3">
@@ -537,31 +633,67 @@
         <v>2.468190564009104</v>
       </c>
       <c r="C3" t="n">
-        <v>2.581362445249754</v>
+        <v>2.589472281019797</v>
       </c>
       <c r="D3" t="n">
-        <v>2.653661411320528</v>
+        <v>3.066289370625425</v>
       </c>
       <c r="E3" t="n">
+        <v>2.828577720844734</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.769117160019671</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2.712442318767745</v>
+      </c>
+      <c r="H3" t="n">
         <v>0.9699308876351251</v>
       </c>
-      <c r="F3" t="n">
-        <v>0.9071580474094858</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.9230254842933501</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.1131718812406497</v>
-      </c>
       <c r="I3" t="n">
-        <v>0.1854708473114237</v>
+        <v>0.9062258530067143</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.06277284022563934</v>
+        <v>0.8561641027395959</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.04690540334177506</v>
+        <v>1.018480999614012</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.8530154002302385</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.751503267021855</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.1212817170106932</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.5980988066163211</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.3603871568356301</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.3009265960105671</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.2442517547586416</v>
+      </c>
+      <c r="S3" t="n">
+        <v>-0.06370503462841082</v>
+      </c>
+      <c r="T3" t="n">
+        <v>-0.1137667848955293</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.04855011197888692</v>
+      </c>
+      <c r="V3" t="n">
+        <v>-0.1169154874048867</v>
+      </c>
+      <c r="W3" t="n">
+        <v>-0.2184276206132701</v>
       </c>
     </row>
     <row r="4">
@@ -574,31 +706,67 @@
         <v>5.713082570197582</v>
       </c>
       <c r="C4" t="n">
-        <v>5.193979145429341</v>
+        <v>5.214058498148367</v>
       </c>
       <c r="D4" t="n">
-        <v>3.342858395300046</v>
+        <v>3.489666168914155</v>
       </c>
       <c r="E4" t="n">
+        <v>3.13657315087518</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.189241431831304</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3.116256800558963</v>
+      </c>
+      <c r="H4" t="n">
         <v>1.292643636471448</v>
       </c>
-      <c r="F4" t="n">
-        <v>1.284241087193813</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.8940198929326667</v>
-      </c>
-      <c r="H4" t="n">
-        <v>-0.5191034247682405</v>
-      </c>
       <c r="I4" t="n">
-        <v>-2.370224174897536</v>
+        <v>1.285187414189988</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.008402549277634952</v>
+        <v>1.004404575526774</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.3986237435387808</v>
+        <v>1.09710563229861</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.8976243119413795</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.8794305171610247</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-0.499024072049215</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-2.223416401283427</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-2.576509419322401</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-2.523841138366278</v>
+      </c>
+      <c r="R4" t="n">
+        <v>-2.596825769638619</v>
+      </c>
+      <c r="S4" t="n">
+        <v>-0.007456222281459146</v>
+      </c>
+      <c r="T4" t="n">
+        <v>-0.2882390609446737</v>
+      </c>
+      <c r="U4" t="n">
+        <v>-0.1955380041728372</v>
+      </c>
+      <c r="V4" t="n">
+        <v>-0.3950193245300681</v>
+      </c>
+      <c r="W4" t="n">
+        <v>-0.4132131193104228</v>
       </c>
     </row>
     <row r="5">
@@ -611,31 +779,67 @@
         <v>13.78807970264317</v>
       </c>
       <c r="C5" t="n">
-        <v>13.44704815314909</v>
+        <v>13.45158414717129</v>
       </c>
       <c r="D5" t="n">
-        <v>12.7678664362851</v>
+        <v>12.51545602290823</v>
       </c>
       <c r="E5" t="n">
+        <v>12.71251798689346</v>
+      </c>
+      <c r="F5" t="n">
+        <v>12.58048641638751</v>
+      </c>
+      <c r="G5" t="n">
+        <v>12.53523161432398</v>
+      </c>
+      <c r="H5" t="n">
         <v>1.097150881057269</v>
       </c>
-      <c r="F5" t="n">
-        <v>1.166577544074186</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.9682467602591793</v>
-      </c>
-      <c r="H5" t="n">
-        <v>-0.3410315494940814</v>
-      </c>
       <c r="I5" t="n">
-        <v>-1.020213266358075</v>
+        <v>1.164234795733726</v>
       </c>
       <c r="J5" t="n">
-        <v>0.06942666301691758</v>
+        <v>1.013350874587507</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.1289041207980894</v>
+        <v>1.018628110968516</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1.000387708345127</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.9771102808825743</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-0.3364955554718883</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-1.272623679734945</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-1.075561715749712</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-1.207593286255666</v>
+      </c>
+      <c r="R5" t="n">
+        <v>-1.252848088319194</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.06708391467645725</v>
+      </c>
+      <c r="T5" t="n">
+        <v>-0.08380000646976216</v>
+      </c>
+      <c r="U5" t="n">
+        <v>-0.07852277008875319</v>
+      </c>
+      <c r="V5" t="n">
+        <v>-0.09676317271214208</v>
+      </c>
+      <c r="W5" t="n">
+        <v>-0.1200406001746944</v>
       </c>
     </row>
     <row r="6">
@@ -648,31 +852,67 @@
         <v>8.304673529463534</v>
       </c>
       <c r="C6" t="n">
-        <v>7.662323184549654</v>
+        <v>7.668290373907366</v>
       </c>
       <c r="D6" t="n">
-        <v>6.038261318870918</v>
+        <v>5.896055479847965</v>
       </c>
       <c r="E6" t="n">
+        <v>5.820702221270763</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5.856413974995616</v>
+      </c>
+      <c r="G6" t="n">
+        <v>6.142760710462269</v>
+      </c>
+      <c r="H6" t="n">
         <v>1.053675744853724</v>
       </c>
-      <c r="F6" t="n">
-        <v>1.064924505132772</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.7937117648211697</v>
-      </c>
-      <c r="H6" t="n">
-        <v>-0.6423503449138792</v>
-      </c>
       <c r="I6" t="n">
-        <v>-2.266412210592615</v>
+        <v>1.063607334170416</v>
       </c>
       <c r="J6" t="n">
-        <v>0.01124876027904786</v>
+        <v>0.8640754600180854</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.2599639800325545</v>
+        <v>0.822392764717888</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.808529699177241</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.7930880846202476</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-0.6363831555561674</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-2.408618049615568</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-2.48397130819277</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-2.448259554467918</v>
+      </c>
+      <c r="R6" t="n">
+        <v>-2.161912819001264</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.009931589316691358</v>
+      </c>
+      <c r="T6" t="n">
+        <v>-0.1896002848356387</v>
+      </c>
+      <c r="U6" t="n">
+        <v>-0.2312829801358361</v>
+      </c>
+      <c r="V6" t="n">
+        <v>-0.2451460456764831</v>
+      </c>
+      <c r="W6" t="n">
+        <v>-0.2605876602334766</v>
       </c>
     </row>
   </sheetData>

</xml_diff>